<commit_message>
additional signatories for PO and RFD
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,76 +219,25 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>kgs</t>
-  </si>
-  <si>
-    <t>pc</t>
-  </si>
-  <si>
-    <t>cans</t>
-  </si>
-  <si>
-    <t>pcs</t>
-  </si>
-  <si>
-    <t>pairs</t>
-  </si>
-  <si>
-    <t>Welding rod 6011</t>
-  </si>
-  <si>
-    <t>Welding rod 6013</t>
-  </si>
-  <si>
-    <t>Welding rod stainless</t>
-  </si>
-  <si>
-    <t>Paint brush 1/2"</t>
-  </si>
-  <si>
-    <t>Paint brush 1"</t>
-  </si>
-  <si>
-    <t>Paint brush 2"</t>
-  </si>
-  <si>
-    <t>Paint brush 3"</t>
-  </si>
-  <si>
-    <t>Paint Brush 4"</t>
-  </si>
-  <si>
-    <t>Sharpening stone (carburandum)</t>
-  </si>
-  <si>
-    <t>Grinding compound G.</t>
-  </si>
-  <si>
-    <t>Grinding compound extra coarse J</t>
-  </si>
-  <si>
-    <t>Metal epoxy (DEVCON)</t>
-  </si>
-  <si>
-    <t>Welding gloves</t>
-  </si>
-  <si>
-    <t>WD40(12.9oz)</t>
-  </si>
-  <si>
-    <t>Steel brush</t>
-  </si>
-  <si>
     <t>Calapan Oriental Mindoro</t>
   </si>
   <si>
-    <t>WAREHOUSE</t>
-  </si>
-  <si>
-    <t>Patrick L.Pineda</t>
-  </si>
-  <si>
-    <t>QUARTERLY CONSUMABLE JULY-SEPTEMBER 2021</t>
+    <t>Jhon Agoncillo</t>
+  </si>
+  <si>
+    <t>OPERATION</t>
+  </si>
+  <si>
+    <t>OPC</t>
+  </si>
+  <si>
+    <t>CHEMICAL FOR WATER TREATMENT</t>
+  </si>
+  <si>
+    <t>Nalco 3 DT 128</t>
+  </si>
+  <si>
+    <t>pails</t>
   </si>
 </sst>
 </file>
@@ -490,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -510,69 +459,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -580,6 +491,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,7 +574,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -922,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,30 +900,30 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -981,14 +931,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -996,136 +946,136 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
       <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
+      <c r="I7" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="26">
-        <v>44454</v>
+      <c r="B8" s="26"/>
+      <c r="C8" s="22">
+        <v>44671</v>
       </c>
       <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="E8" s="23"/>
       <c r="H8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
+      <c r="I8" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="26">
-        <v>44455</v>
+      <c r="B9" s="26"/>
+      <c r="C9" s="22">
+        <v>44671</v>
       </c>
       <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
+      <c r="E9" s="23"/>
       <c r="H9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="24"/>
+      <c r="I9" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="24"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="24"/>
+      <c r="C11" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="30"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
+      <c r="C12" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1140,438 +1090,125 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="13" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="J13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
       <c r="B14" s="11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D14" s="11"/>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="10">
         <v>0</v>
       </c>
-      <c r="J14" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K14" s="28"/>
+      <c r="J14" s="22">
+        <v>44701</v>
+      </c>
+      <c r="K14" s="23"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>2</v>
-      </c>
-      <c r="B15" s="11">
-        <v>5</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="10">
-        <v>0</v>
-      </c>
-      <c r="J15" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K15" s="28"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>3</v>
-      </c>
-      <c r="B16" s="11">
-        <v>2</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="10">
-        <v>0</v>
-      </c>
-      <c r="J16" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K16" s="28"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>4</v>
-      </c>
-      <c r="B17" s="11">
-        <v>1</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="10">
-        <v>0</v>
-      </c>
-      <c r="J17" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K17" s="28"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>5</v>
-      </c>
-      <c r="B18" s="11">
-        <v>1</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="10">
-        <v>0</v>
-      </c>
-      <c r="J18" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K18" s="28"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>6</v>
-      </c>
-      <c r="B19" s="11">
-        <v>1</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="10">
-        <v>0</v>
-      </c>
-      <c r="J19" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K19" s="28"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>7</v>
-      </c>
-      <c r="B20" s="11">
-        <v>1</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="10">
-        <v>0</v>
-      </c>
-      <c r="J20" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K20" s="28"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>8</v>
-      </c>
-      <c r="B21" s="11">
-        <v>1</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="10">
-        <v>0</v>
-      </c>
-      <c r="J21" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K21" s="28"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>9</v>
-      </c>
-      <c r="B22" s="11">
-        <v>1</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="10">
-        <v>0</v>
-      </c>
-      <c r="J22" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K22" s="28"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>10</v>
-      </c>
-      <c r="B23" s="11">
-        <v>2</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="10">
-        <v>0</v>
-      </c>
-      <c r="J23" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K23" s="28"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>11</v>
-      </c>
-      <c r="B24" s="11">
-        <v>2</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="10">
-        <v>0</v>
-      </c>
-      <c r="J24" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K24" s="28"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>12</v>
-      </c>
-      <c r="B25" s="11">
-        <v>2</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="10">
-        <v>0</v>
-      </c>
-      <c r="J25" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K25" s="28"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>13</v>
-      </c>
-      <c r="B26" s="11">
-        <v>2</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="10">
-        <v>0</v>
-      </c>
-      <c r="J26" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K26" s="28"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>14</v>
-      </c>
-      <c r="B27" s="11">
-        <v>2</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="10">
-        <v>0</v>
-      </c>
-      <c r="J27" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K27" s="28"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
-        <v>15</v>
-      </c>
-      <c r="B28" s="11">
-        <v>2</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="10">
-        <v>0</v>
-      </c>
-      <c r="J28" s="26">
-        <v>44484</v>
-      </c>
-      <c r="K28" s="28"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
+  <mergeCells count="23">
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1582,6 +1219,19 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>